<commit_message>
#nghia.le sửa lại tên thư mục, update db
update on 12:21 13/2/2020 sửa lại tên thư mục và chỉnh sửa lại db mới
</commit_message>
<xml_diff>
--- a/docs/Database-log/noteDBLog.xlsx
+++ b/docs/Database-log/noteDBLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\real_estate\docs\Database-log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FF4349-443D-457F-802E-BBAAFEA54DE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB1DF21-78A1-421D-82FE-BB5A78838AE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Ngày</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Vẽ lại db bằng workbench, có comment và set datatype các trường dữ liệu</t>
+  </si>
+  <si>
+    <t>13/2/2020</t>
+  </si>
+  <si>
+    <t>Sửa lại các khóa ngoại, bỏ note hình ảnh hợp đồng, sửa tên folder db</t>
   </si>
 </sst>
 </file>
@@ -393,7 +399,15 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>